<commit_message>
BEST? done, now opti
</commit_message>
<xml_diff>
--- a/data/5_results/no_prompt/result_no_prompt_1.xlsx
+++ b/data/5_results/no_prompt/result_no_prompt_1.xlsx
@@ -507,22 +507,22 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>0,405</t>
+          <t>0,517</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>0,500</t>
+          <t>0,682</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>0,448</t>
+          <t>0,588</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>0,341</t>
+          <t>0,951</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -553,22 +553,22 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>0,436</t>
+          <t>0,630</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>0,500</t>
+          <t>0,773</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>0,466</t>
+          <t>0,694</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>0,386</t>
+          <t>0,970</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -599,22 +599,22 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>0,371</t>
+          <t>0,448</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>0,464</t>
+          <t>0,591</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>0,413</t>
+          <t>0,510</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>0,295</t>
+          <t>0,930</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -645,22 +645,22 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>0,395</t>
+          <t>0,556</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>0,469</t>
+          <t>0,714</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>0,429</t>
+          <t>0,625</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>0,341</t>
+          <t>0,922</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -691,22 +691,22 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>0,290</t>
+          <t>0,360</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>0,321</t>
+          <t>0,409</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>0,305</t>
+          <t>0,383</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>0,205</t>
+          <t>0,974</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -737,22 +737,22 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>0,267</t>
+          <t>0,320</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>0,296</t>
+          <t>0,364</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>0,281</t>
+          <t>0,340</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>0,182</t>
+          <t>1,000</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -798,7 +798,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>0,000</t>
+          <t>0,872</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -829,22 +829,22 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>0,086</t>
+          <t>0,188</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>0,097</t>
+          <t>0,250</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>0,091</t>
+          <t>0,214</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>0,068</t>
+          <t>0,971</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -875,22 +875,22 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>0,195</t>
+          <t>0,533</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>0,216</t>
+          <t>0,727</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>0,205</t>
+          <t>0,615</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>0,182</t>
+          <t>0,943</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -921,22 +921,22 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>0,162</t>
+          <t>0,462</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>0,162</t>
+          <t>0,462</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>0,162</t>
+          <t>0,462</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>0,136</t>
+          <t>0,955</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -967,22 +967,22 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>0,162</t>
+          <t>0,462</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>0,162</t>
+          <t>0,462</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>0,162</t>
+          <t>0,462</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>0,136</t>
+          <t>0,948</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -1013,22 +1013,22 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>0,158</t>
+          <t>0,462</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>0,162</t>
+          <t>0,500</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>0,160</t>
+          <t>0,480</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>0,136</t>
+          <t>0,953</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -1059,22 +1059,22 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>0,135</t>
+          <t>0,385</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>0,139</t>
+          <t>0,417</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>0,137</t>
+          <t>0,400</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>0,114</t>
+          <t>0,941</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -1105,22 +1105,22 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>0,262</t>
+          <t>0,524</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>0,324</t>
+          <t>0,846</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>0,289</t>
+          <t>0,647</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>0,250</t>
+          <t>0,821</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -1151,22 +1151,22 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>0,128</t>
+          <t>0,333</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>0,147</t>
+          <t>0,500</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>0,137</t>
+          <t>0,400</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>0,114</t>
+          <t>0,958</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -1197,22 +1197,22 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>0,132</t>
+          <t>0,294</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>0,156</t>
+          <t>0,455</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>0,143</t>
+          <t>0,357</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>0,114</t>
+          <t>0,920</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -1243,22 +1243,22 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>0,051</t>
+          <t>0,154</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>0,061</t>
+          <t>0,286</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>0,056</t>
+          <t>0,200</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>0,045</t>
+          <t>0,957</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -1289,22 +1289,22 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>0,171</t>
+          <t>0,583</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>0,179</t>
+          <t>0,700</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>0,175</t>
+          <t>0,636</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>0,159</t>
+          <t>0,642</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -1335,22 +1335,22 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>0,122</t>
+          <t>0,417</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>0,135</t>
+          <t>0,625</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>0,128</t>
+          <t>0,500</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>0,114</t>
+          <t>0,684</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -1381,22 +1381,22 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>0,048</t>
+          <t>0,154</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>0,061</t>
+          <t>0,500</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>0,053</t>
+          <t>0,235</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>0,045</t>
+          <t>0,813</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -1427,22 +1427,22 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>0,026</t>
+          <t>0,250</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>0,024</t>
+          <t>0,167</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>0,025</t>
+          <t>0,200</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>0,023</t>
+          <t>0,909</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -1473,22 +1473,22 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>0,023</t>
+          <t>0,333</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>0,024</t>
+          <t>1,000</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>0,023</t>
+          <t>0,500</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>0,023</t>
+          <t>0,333</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -1534,7 +1534,7 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>0,000</t>
+          <t>0,913</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -1611,22 +1611,22 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>0,025</t>
+          <t>0,143</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>0,026</t>
+          <t>0,200</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>0,026</t>
+          <t>0,167</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>0,023</t>
+          <t>1,000</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -1657,22 +1657,22 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>0,026</t>
+          <t>1,000</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>0,023</t>
+          <t>0,167</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>0,024</t>
+          <t>0,286</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>0,023</t>
+          <t>0,167</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -1718,7 +1718,7 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>0,000</t>
+          <t>1,000</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -1749,22 +1749,22 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>0,025</t>
+          <t>0,100</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>0,029</t>
+          <t>0,200</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>0,027</t>
+          <t>0,133</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>0,023</t>
+          <t>1,000</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -1795,22 +1795,22 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>0,047</t>
+          <t>0,222</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>0,054</t>
+          <t>0,667</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>0,050</t>
+          <t>0,333</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>0,045</t>
+          <t>0,836</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -1887,22 +1887,22 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>0,025</t>
+          <t>0,125</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>0,027</t>
+          <t>0,200</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>0,026</t>
+          <t>0,154</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>0,023</t>
+          <t>1,000</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -1933,22 +1933,22 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>0,023</t>
+          <t>1,000</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>0,023</t>
+          <t>1,000</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>0,023</t>
+          <t>1,000</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>0,023</t>
+          <t>1,000</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -2025,22 +2025,22 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>0,024</t>
+          <t>1,000</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>0,023</t>
+          <t>0,250</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>0,024</t>
+          <t>0,400</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>0,023</t>
+          <t>0,250</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -2071,22 +2071,22 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>0,024</t>
+          <t>0,333</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>0,024</t>
+          <t>0,250</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>0,024</t>
+          <t>0,286</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>0,023</t>
+          <t>1,000</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -2132,7 +2132,7 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>0,000</t>
+          <t>1,000</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -2178,7 +2178,7 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>0,000</t>
+          <t>1,000</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -2224,7 +2224,7 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>0,000</t>
+          <t>1,000</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -2255,22 +2255,22 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>0,024</t>
+          <t>0,200</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>0,025</t>
+          <t>0,333</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>0,024</t>
+          <t>0,250</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>0,023</t>
+          <t>1,000</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -2393,22 +2393,22 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>0,048</t>
+          <t>0,333</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>0,050</t>
+          <t>0,500</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>0,049</t>
+          <t>0,400</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>0,045</t>
+          <t>1,000</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -2454,7 +2454,7 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>0,000</t>
+          <t>1,000</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -2485,22 +2485,22 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>0,024</t>
+          <t>0,167</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>0,026</t>
+          <t>0,333</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>0,025</t>
+          <t>0,222</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>0,023</t>
+          <t>1,000</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -2592,7 +2592,7 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>0,000</t>
+          <t>1,000</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -2638,7 +2638,7 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>0,000</t>
+          <t>1,000</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -2874,7 +2874,7 @@
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>0,000</t>
+          <t>0,243</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
@@ -4366,22 +4366,22 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>0,078</t>
+          <t>0,222</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>0,063</t>
+          <t>0,623</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>0,201</t>
+          <t>0,390</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>0,157</t>
+          <t>0,850</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
opti 70 15 15
</commit_message>
<xml_diff>
--- a/data/5_results/no_prompt/result_no_prompt_1.xlsx
+++ b/data/5_results/no_prompt/result_no_prompt_1.xlsx
@@ -507,22 +507,22 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>0,485</t>
+          <t>0,449</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>0,640</t>
+          <t>0,880</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>0,552</t>
+          <t>0,595</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>0,977</t>
+          <t>0,873</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -536,13 +536,13 @@
         </is>
       </c>
       <c r="H2" t="n">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="I2" t="n">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="J2" t="n">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3">
@@ -553,22 +553,22 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>0,483</t>
+          <t>0,512</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>0,583</t>
+          <t>0,917</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>0,528</t>
+          <t>0,657</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>0,966</t>
+          <t>0,887</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -582,13 +582,13 @@
         </is>
       </c>
       <c r="H3" t="n">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="I3" t="n">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="J3" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4">
@@ -599,22 +599,22 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>0,438</t>
+          <t>0,429</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>0,560</t>
+          <t>0,960</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>0,491</t>
+          <t>0,593</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>0,949</t>
+          <t>0,702</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -628,13 +628,13 @@
         </is>
       </c>
       <c r="H4" t="n">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="I4" t="n">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="J4" t="n">
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5">
@@ -650,17 +650,17 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>0,560</t>
+          <t>0,840</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>0,528</t>
+          <t>0,627</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>0,975</t>
+          <t>0,871</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -674,13 +674,13 @@
         </is>
       </c>
       <c r="H5" t="n">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="I5" t="n">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="J5" t="n">
-        <v>11</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6">
@@ -691,17 +691,17 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>0,294</t>
+          <t>0,250</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>0,185</t>
+          <t>0,222</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>0,227</t>
+          <t>0,235</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -711,22 +711,22 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>27,000</t>
+          <t>36,000</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>0,39</t>
+          <t>0,52</t>
         </is>
       </c>
       <c r="H6" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="I6" t="n">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="J6" t="n">
-        <v>22</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7">
@@ -737,42 +737,42 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>0,353</t>
+          <t>0,312</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>0,214</t>
+          <t>0,294</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>0,267</t>
+          <t>0,303</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>0,987</t>
+          <t>1,000</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>28,000</t>
+          <t>34,000</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>0,41</t>
+          <t>0,49</t>
         </is>
       </c>
       <c r="H7" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="I7" t="n">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="J7" t="n">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8">
@@ -783,22 +783,22 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>0,000</t>
+          <t>0,091</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>0,000</t>
+          <t>0,200</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>0,000</t>
+          <t>0,125</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>0,862</t>
+          <t>0,902</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -812,13 +812,13 @@
         </is>
       </c>
       <c r="H8" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I8" t="n">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="J8" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9">
@@ -829,42 +829,42 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>0,400</t>
+          <t>0,632</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>0,111</t>
+          <t>0,632</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>0,174</t>
+          <t>0,632</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>0,909</t>
+          <t>0,767</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>18,000</t>
+          <t>19,000</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>0,26</t>
+          <t>0,28</t>
         </is>
       </c>
       <c r="H9" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="I9" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="J9" t="n">
-        <v>16</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10">
@@ -890,7 +890,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>0,779</t>
+          <t>0,771</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -907,7 +907,7 @@
         <v>0</v>
       </c>
       <c r="I10" t="n">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="J10" t="n">
         <v>2</v>
@@ -921,17 +921,17 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>0,000</t>
+          <t>0,158</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>0,000</t>
+          <t>0,500</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>0,000</t>
+          <t>0,240</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -950,13 +950,13 @@
         </is>
       </c>
       <c r="H11" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I11" t="n">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="J11" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12">
@@ -967,17 +967,17 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>0,000</t>
+          <t>0,158</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>0,000</t>
+          <t>0,500</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>0,000</t>
+          <t>0,240</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -996,13 +996,13 @@
         </is>
       </c>
       <c r="H12" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I12" t="n">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="J12" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13">
@@ -1013,17 +1013,17 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>0,000</t>
+          <t>0,211</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>0,000</t>
+          <t>0,444</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>0,000</t>
+          <t>0,286</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -1042,13 +1042,13 @@
         </is>
       </c>
       <c r="H13" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I13" t="n">
+        <v>15</v>
+      </c>
+      <c r="J13" t="n">
         <v>5</v>
-      </c>
-      <c r="J13" t="n">
-        <v>9</v>
       </c>
     </row>
     <row r="14">
@@ -1059,17 +1059,17 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>0,000</t>
+          <t>0,211</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>0,000</t>
+          <t>0,444</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>0,000</t>
+          <t>0,286</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -1088,13 +1088,13 @@
         </is>
       </c>
       <c r="H14" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I14" t="n">
+        <v>15</v>
+      </c>
+      <c r="J14" t="n">
         <v>5</v>
-      </c>
-      <c r="J14" t="n">
-        <v>9</v>
       </c>
     </row>
     <row r="15">
@@ -1105,22 +1105,22 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>0,071</t>
+          <t>0,421</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>0,077</t>
+          <t>0,615</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>0,074</t>
+          <t>0,500</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>0,209</t>
+          <t>0,794</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -1134,13 +1134,13 @@
         </is>
       </c>
       <c r="H15" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="I15" t="n">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="J15" t="n">
-        <v>12</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16">
@@ -1151,7 +1151,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>0,033</t>
+          <t>0,043</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -1161,12 +1161,12 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>0,062</t>
+          <t>0,080</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>0,797</t>
+          <t>0,794</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -1183,7 +1183,7 @@
         <v>1</v>
       </c>
       <c r="I16" t="n">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="J16" t="n">
         <v>1</v>
@@ -1197,22 +1197,22 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>0,000</t>
+          <t>0,667</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>0,000</t>
+          <t>0,933</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>0,000</t>
+          <t>0,778</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>0,884</t>
+          <t>0,971</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -1226,13 +1226,13 @@
         </is>
       </c>
       <c r="H17" t="n">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="I17" t="n">
         <v>7</v>
       </c>
       <c r="J17" t="n">
-        <v>15</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18">
@@ -1275,7 +1275,7 @@
         <v>0</v>
       </c>
       <c r="I18" t="n">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="J18" t="n">
         <v>0</v>
@@ -1289,22 +1289,22 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>0,038</t>
+          <t>0,143</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>0,500</t>
+          <t>1,000</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>0,071</t>
+          <t>0,250</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>0,393</t>
+          <t>0,143</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -1318,13 +1318,13 @@
         </is>
       </c>
       <c r="H19" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I19" t="n">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="J19" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20">
@@ -1335,22 +1335,22 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>0,038</t>
+          <t>0,133</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>0,500</t>
+          <t>1,000</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>0,071</t>
+          <t>0,235</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>0,393</t>
+          <t>0,133</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -1364,13 +1364,13 @@
         </is>
       </c>
       <c r="H20" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I20" t="n">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="J20" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21">
@@ -1381,22 +1381,22 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>0,000</t>
+          <t>0,062</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>0,000</t>
+          <t>0,250</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>0,000</t>
+          <t>0,100</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>0,181</t>
+          <t>0,248</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -1410,13 +1410,13 @@
         </is>
       </c>
       <c r="H21" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I21" t="n">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="J21" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="22">
@@ -1427,17 +1427,17 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
+          <t>0,400</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
           <t>0,500</t>
         </is>
       </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>0,182</t>
-        </is>
-      </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>0,267</t>
+          <t>0,444</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
@@ -1447,22 +1447,22 @@
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>11,000</t>
+          <t>12,000</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>0,16</t>
+          <t>0,17</t>
         </is>
       </c>
       <c r="H22" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="I22" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="J22" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="23">
@@ -1488,7 +1488,7 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>0,784</t>
+          <t>0,948</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -1505,7 +1505,7 @@
         <v>0</v>
       </c>
       <c r="I23" t="n">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="J23" t="n">
         <v>1</v>
@@ -1519,42 +1519,42 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>0,000</t>
+          <t>0,400</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>0,000</t>
+          <t>0,462</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>0,000</t>
+          <t>0,429</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>0,914</t>
+          <t>0,964</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>12,000</t>
+          <t>13,000</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>0,17</t>
+          <t>0,19</t>
         </is>
       </c>
       <c r="H24" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="I24" t="n">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="J24" t="n">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="25">
@@ -1580,7 +1580,7 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>0,893</t>
+          <t>0,952</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -1597,7 +1597,7 @@
         <v>0</v>
       </c>
       <c r="I25" t="n">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="J25" t="n">
         <v>1</v>
@@ -1611,17 +1611,17 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>0,250</t>
+          <t>0,500</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>0,286</t>
+          <t>0,571</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>0,267</t>
+          <t>0,533</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
@@ -1640,13 +1640,13 @@
         </is>
       </c>
       <c r="H26" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I26" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="J26" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="27">
@@ -1657,24 +1657,24 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
+          <t>0,222</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>0,667</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>0,333</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
           <t>1,000</t>
         </is>
       </c>
-      <c r="C27" t="inlineStr">
-        <is>
-          <t>0,333</t>
-        </is>
-      </c>
-      <c r="D27" t="inlineStr">
-        <is>
-          <t>0,500</t>
-        </is>
-      </c>
-      <c r="E27" t="inlineStr">
-        <is>
-          <t>0,333</t>
-        </is>
-      </c>
       <c r="F27" t="inlineStr">
         <is>
           <t>3,000</t>
@@ -1686,13 +1686,13 @@
         </is>
       </c>
       <c r="H27" t="n">
+        <v>2</v>
+      </c>
+      <c r="I27" t="n">
+        <v>7</v>
+      </c>
+      <c r="J27" t="n">
         <v>1</v>
-      </c>
-      <c r="I27" t="n">
-        <v>0</v>
-      </c>
-      <c r="J27" t="n">
-        <v>2</v>
       </c>
     </row>
     <row r="28">
@@ -1703,17 +1703,17 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>0,000</t>
+          <t>0,062</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>0,000</t>
+          <t>0,250</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>0,000</t>
+          <t>0,100</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
@@ -1732,13 +1732,13 @@
         </is>
       </c>
       <c r="H28" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I28" t="n">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="J28" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="29">
@@ -1749,22 +1749,22 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>0,000</t>
+          <t>0,316</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>0,000</t>
+          <t>0,462</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>0,000</t>
+          <t>0,375</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>0,548</t>
+          <t>1,000</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -1778,13 +1778,13 @@
         </is>
       </c>
       <c r="H29" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="I29" t="n">
+        <v>13</v>
+      </c>
+      <c r="J29" t="n">
         <v>7</v>
-      </c>
-      <c r="J29" t="n">
-        <v>13</v>
       </c>
     </row>
     <row r="30">
@@ -1795,22 +1795,22 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>0,000</t>
+          <t>0,583</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>0,000</t>
+          <t>0,636</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>0,000</t>
+          <t>0,609</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>0,000</t>
+          <t>1,000</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -1824,13 +1824,13 @@
         </is>
       </c>
       <c r="H30" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="I30" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J30" t="n">
-        <v>11</v>
+        <v>4</v>
       </c>
     </row>
     <row r="31">
@@ -1919,7 +1919,7 @@
         <v>0</v>
       </c>
       <c r="I32" t="n">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="J32" t="n">
         <v>2</v>
@@ -1933,22 +1933,22 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>0,400</t>
+          <t>0,200</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>0,667</t>
+          <t>1,000</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>0,500</t>
+          <t>0,333</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>1,000</t>
+          <t>0,200</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -1962,13 +1962,13 @@
         </is>
       </c>
       <c r="H33" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I33" t="n">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="J33" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34">
@@ -1979,22 +1979,22 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>0,000</t>
+          <t>0,286</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>0,000</t>
+          <t>1,000</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>0,000</t>
+          <t>0,444</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>0,000</t>
+          <t>0,286</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -2008,13 +2008,13 @@
         </is>
       </c>
       <c r="H34" t="n">
+        <v>2</v>
+      </c>
+      <c r="I34" t="n">
+        <v>5</v>
+      </c>
+      <c r="J34" t="n">
         <v>0</v>
-      </c>
-      <c r="I34" t="n">
-        <v>0</v>
-      </c>
-      <c r="J34" t="n">
-        <v>2</v>
       </c>
     </row>
     <row r="35">
@@ -2025,22 +2025,22 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>0,000</t>
+          <t>0,100</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>0,000</t>
+          <t>1,000</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>0,000</t>
+          <t>0,182</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>0,000</t>
+          <t>0,100</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -2054,13 +2054,13 @@
         </is>
       </c>
       <c r="H35" t="n">
+        <v>1</v>
+      </c>
+      <c r="I35" t="n">
+        <v>9</v>
+      </c>
+      <c r="J35" t="n">
         <v>0</v>
-      </c>
-      <c r="I35" t="n">
-        <v>0</v>
-      </c>
-      <c r="J35" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="36">
@@ -2071,17 +2071,17 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>0,000</t>
+          <t>0,400</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>0,000</t>
+          <t>0,462</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>0,000</t>
+          <t>0,429</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
@@ -2091,22 +2091,22 @@
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>12,000</t>
+          <t>13,000</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>0,17</t>
+          <t>0,19</t>
         </is>
       </c>
       <c r="H36" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="I36" t="n">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="J36" t="n">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="37">
@@ -2163,17 +2163,17 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>0,200</t>
+          <t>0,250</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>0,250</t>
+          <t>0,111</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>0,222</t>
+          <t>0,154</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
@@ -2183,74 +2183,68 @@
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>8,000</t>
+          <t>9,000</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>0,12</t>
+          <t>0,13</t>
         </is>
       </c>
       <c r="H38" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I38" t="n">
+        <v>3</v>
+      </c>
+      <c r="J38" t="n">
         <v>8</v>
-      </c>
-      <c r="J38" t="n">
-        <v>6</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Open Spring</t>
+          <t>open spring</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0,000</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0,000</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0,000</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0,000</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0,000</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H39" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I39" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="J39" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+          <t>0,00</t>
+        </is>
+      </c>
+      <c r="H39" t="n">
+        <v>0</v>
+      </c>
+      <c r="I39" t="n">
+        <v>6</v>
+      </c>
+      <c r="J39" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="40">
@@ -2261,17 +2255,17 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>0,167</t>
+          <t>0,000</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>0,333</t>
+          <t>0,000</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>0,222</t>
+          <t>0,000</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
@@ -2281,22 +2275,22 @@
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>3,000</t>
+          <t>4,000</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>0,04</t>
+          <t>0,06</t>
         </is>
       </c>
       <c r="H40" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I40" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="J40" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="41">
@@ -2405,17 +2399,17 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>0,167</t>
+          <t>0,000</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>0,333</t>
+          <t>0,000</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>0,222</t>
+          <t>0,000</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
@@ -2425,22 +2419,22 @@
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>3,000</t>
+          <t>4,000</t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>0,04</t>
+          <t>0,06</t>
         </is>
       </c>
       <c r="H43" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I43" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="J43" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="44">
@@ -2471,12 +2465,12 @@
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>4,000</t>
+          <t>6,000</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>0,06</t>
+          <t>0,09</t>
         </is>
       </c>
       <c r="H44" t="n">
@@ -2486,7 +2480,7 @@
         <v>0</v>
       </c>
       <c r="J44" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="45">
@@ -2497,22 +2491,22 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>0,000</t>
+          <t>0,545</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>0,000</t>
+          <t>0,545</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>0,000</t>
+          <t>0,545</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>0,000</t>
+          <t>0,949</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -2526,13 +2520,13 @@
         </is>
       </c>
       <c r="H45" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="I45" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J45" t="n">
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
     <row r="46">
@@ -2794,7 +2788,7 @@
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>0,000</t>
+          <t>0,212</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -2811,7 +2805,7 @@
         <v>0</v>
       </c>
       <c r="I51" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J51" t="n">
         <v>2</v>
@@ -2990,7 +2984,7 @@
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>0,000</t>
+          <t>1,000</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
@@ -3007,7 +3001,7 @@
         <v>0</v>
       </c>
       <c r="I55" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J55" t="n">
         <v>1</v>
@@ -4408,22 +4402,22 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>0,101</t>
+          <t>0,220</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>0,572</t>
+          <t>0,631</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>0,206</t>
+          <t>0,392</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>0,770</t>
+          <t>0,832</t>
         </is>
       </c>
     </row>
@@ -4501,7 +4495,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>94</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6">

</xml_diff>